<commit_message>
add more if conditions
added startsWith, endsWith, greaterThan, greaterThanOrEqual, lessThan,
lessThanOrEqual
</commit_message>
<xml_diff>
--- a/examples/milestone_5/issue_22/testcase.xlsx
+++ b/examples/milestone_5/issue_22/testcase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="66">
   <si>
     <t>No</t>
   </si>
@@ -155,6 +155,69 @@
   </si>
   <si>
     <t>ssh</t>
+  </si>
+  <si>
+    <t>Test If StartsWith positive</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>startsWith</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>Test If StartsWith negative</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>Test If EndsWith positive</t>
+  </si>
+  <si>
+    <t>endsWith</t>
+  </si>
+  <si>
+    <t>Test If EndsWith negative</t>
+  </si>
+  <si>
+    <t>Test If GreaterThan positive</t>
+  </si>
+  <si>
+    <t>greaterThan</t>
+  </si>
+  <si>
+    <t>Test If GreaterThan negative</t>
+  </si>
+  <si>
+    <t>Test If LessThan positive</t>
+  </si>
+  <si>
+    <t>Test If LessThan negative</t>
+  </si>
+  <si>
+    <t>lessThan</t>
+  </si>
+  <si>
+    <t>Test If GreaterThanOrEqual positive</t>
+  </si>
+  <si>
+    <t>Test If GreaterThanOrEqual negative</t>
+  </si>
+  <si>
+    <t>greaterThanOrEqual</t>
+  </si>
+  <si>
+    <t>lessThanOrEqual</t>
+  </si>
+  <si>
+    <t>Test If LessThanOrEqual positive</t>
+  </si>
+  <si>
+    <t>Test If LessThanOrEqual negative</t>
   </si>
 </sst>
 </file>
@@ -498,17 +561,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -754,86 +818,422 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1">
         <v>2</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="3" t="s">
+      <c r="D28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -845,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
#115 add ifExpr and runLoopEnd
</commit_message>
<xml_diff>
--- a/examples/milestone_5/issue_22/testcase.xlsx
+++ b/examples/milestone_5/issue_22/testcase.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
   <si>
     <t>No</t>
   </si>
@@ -224,6 +224,27 @@
   </si>
   <si>
     <t>notExistRule</t>
+  </si>
+  <si>
+    <t>ifExpr</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>vars["apple"] == 3</t>
+  </si>
+  <si>
+    <t>runLoopEnd</t>
+  </si>
+  <si>
+    <t>Test RunLoop start end step</t>
+  </si>
+  <si>
+    <t>Test If Expr positive</t>
+  </si>
+  <si>
+    <t>Test If Expr negative</t>
   </si>
 </sst>
 </file>
@@ -567,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1187,83 +1208,275 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2</v>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="1">
-        <v>3</v>
+      <c r="B27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1">
+      <c r="F27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="1">
         <v>2</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="3"/>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="3" t="s">
-        <v>42</v>
+      <c r="F29" s="1">
+        <v>2</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>5</v>
+      </c>
+      <c r="H34" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5</v>
+      </c>
+      <c r="H35" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>5</v>
+      </c>
+      <c r="H36" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>